<commit_message>
Bug fix: ability to parse merged header cells horizontally
</commit_message>
<xml_diff>
--- a/src/test/resources/spreadsheet_examples/header_cells.xlsx
+++ b/src/test/resources/spreadsheet_examples/header_cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\stefbg\projects\refinery\src\test\resources\spreadsheet_examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\stefbg\projects\refinery\src\test\resources\spreadsheet_examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790A163B-39C4-4D43-BE9F-19DE1C3D27B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F08955B-F8BF-4A6B-B0B3-6A21CE28DEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8FC5C0BD-89C0-414B-A5CA-9C6500A5AC53}"/>
+    <workbookView xWindow="-23136" yWindow="-3078" windowWidth="23232" windowHeight="12432" xr2:uid="{8FC5C0BD-89C0-414B-A5CA-9C6500A5AC53}"/>
   </bookViews>
   <sheets>
     <sheet name="header_cells" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>mergedHeader2</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>regexHeader</t>
+  </si>
+  <si>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>group2</t>
   </si>
 </sst>
 </file>
@@ -90,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -100,6 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,24 +421,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C909622B-DAA7-1243-9E83-94FC53503F77}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17.08203125" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" customWidth="1"/>
+    <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="10" max="10" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -453,17 +461,62 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="1"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
       <c r="J2" s="5"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="9">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
   </mergeCells>

</xml_diff>